<commit_message>
Added correct fuel values to the car info
</commit_message>
<xml_diff>
--- a/Fuel Sheet of the cars.xlsx
+++ b/Fuel Sheet of the cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\source\repos\Fuel-App-ACC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{657393D3-837F-4FB6-B9EB-7CC68D0F116B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1A9774-5D5A-42A4-8A59-2EFDB03A8198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F74DF76B-50E2-4403-BFAE-32475E89D87E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>AMR_V12_Vantage_GT3,</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Lexus_RC_F_GT3,</t>
+  </si>
+  <si>
+    <t>*2018-19 same amounts</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABF09C5-F3F6-404B-95DF-A26B4215ABA0}">
-  <dimension ref="B1:C23"/>
+  <dimension ref="B1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +598,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
@@ -603,7 +606,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
@@ -611,7 +614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
@@ -619,7 +622,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
@@ -627,15 +630,18 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C21">
         <v>120</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
@@ -643,7 +649,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>21</v>
       </c>

</xml_diff>